<commit_message>
all changes and correlations strat desing uo
</commit_message>
<xml_diff>
--- a/INTRADAY-DATA/YIELDS-DATA/10YYIELD-DATA/10YYIELD_6M_240.xlsx
+++ b/INTRADAY-DATA/YIELDS-DATA/10YYIELD-DATA/10YYIELD_6M_240.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgentUser\AppData\Local\Temp\CitrixClient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertozuniga/Desktop/kickstartstrategies/INTRADAY-DATA/YIELDS-DATA/10YYIELD-DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A85DC0-D17C-8745-B8D8-779B457E5B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="1320" windowWidth="21220" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,20 +348,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B189"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:B189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44728.583333333336</v>
       </c>
@@ -376,7 +377,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44727.583333333336</v>
       </c>
@@ -384,7 +385,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44726.583333333336</v>
       </c>
@@ -392,7 +393,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44725.583333333336</v>
       </c>
@@ -400,7 +401,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44722.583333333336</v>
       </c>
@@ -408,7 +409,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44721.583333333336</v>
       </c>
@@ -416,7 +417,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44720.583333333336</v>
       </c>
@@ -424,7 +425,7 @@
         <v>3.03</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44719.583333333336</v>
       </c>
@@ -432,7 +433,7 @@
         <v>2.98</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44718.583333333336</v>
       </c>
@@ -440,7 +441,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44715.583333333336</v>
       </c>
@@ -448,7 +449,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44714.583333333336</v>
       </c>
@@ -456,7 +457,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44713.583333333336</v>
       </c>
@@ -464,7 +465,7 @@
         <v>2.94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44712.583333333336</v>
       </c>
@@ -472,7 +473,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44708.583333333336</v>
       </c>
@@ -480,7 +481,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44707.583333333336</v>
       </c>
@@ -488,7 +489,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44706.583333333336</v>
       </c>
@@ -496,7 +497,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44705.583333333336</v>
       </c>
@@ -504,7 +505,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44704.583333333336</v>
       </c>
@@ -512,7 +513,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44701.583333333336</v>
       </c>
@@ -520,7 +521,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44700.583333333336</v>
       </c>
@@ -528,7 +529,7 @@
         <v>2.84</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44699.583333333336</v>
       </c>
@@ -536,7 +537,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44698.583333333336</v>
       </c>
@@ -544,7 +545,7 @@
         <v>2.98</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44697.583333333336</v>
       </c>
@@ -552,7 +553,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44694.583333333336</v>
       </c>
@@ -560,7 +561,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44693.583333333336</v>
       </c>
@@ -568,7 +569,7 @@
         <v>2.84</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44692.541666666664</v>
       </c>
@@ -576,7 +577,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44691.541666666664</v>
       </c>
@@ -584,7 +585,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44690.541666666664</v>
       </c>
@@ -592,7 +593,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44687.541666666664</v>
       </c>
@@ -600,7 +601,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44686.541666666664</v>
       </c>
@@ -608,7 +609,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44685.541666666664</v>
       </c>
@@ -616,7 +617,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44684.541666666664</v>
       </c>
@@ -624,7 +625,7 @@
         <v>2.97</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44683.541666666664</v>
       </c>
@@ -632,7 +633,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44680.541666666664</v>
       </c>
@@ -640,7 +641,7 @@
         <v>2.89</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44679.541666666664</v>
       </c>
@@ -648,7 +649,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>44678.541666666664</v>
       </c>
@@ -656,7 +657,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>44677.541666666664</v>
       </c>
@@ -664,7 +665,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>44676.541666666664</v>
       </c>
@@ -672,7 +673,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>44673.541666666664</v>
       </c>
@@ -680,7 +681,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44672.541666666664</v>
       </c>
@@ -688,7 +689,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44671.541666666664</v>
       </c>
@@ -696,7 +697,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44670.541666666664</v>
       </c>
@@ -704,7 +705,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44669.541666666664</v>
       </c>
@@ -712,7 +713,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44665.541666666664</v>
       </c>
@@ -720,7 +721,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44664.541666666664</v>
       </c>
@@ -728,7 +729,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44663.541666666664</v>
       </c>
@@ -736,7 +737,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44662.583333333336</v>
       </c>
@@ -744,7 +745,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44659.583333333336</v>
       </c>
@@ -752,7 +753,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>44658.583333333336</v>
       </c>
@@ -760,7 +761,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>44657.583333333336</v>
       </c>
@@ -768,7 +769,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>44656.583333333336</v>
       </c>
@@ -776,7 +777,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>44655.583333333336</v>
       </c>
@@ -784,7 +785,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>44652.583333333336</v>
       </c>
@@ -792,7 +793,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>44651.583333333336</v>
       </c>
@@ -800,7 +801,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>44650.583333333336</v>
       </c>
@@ -808,7 +809,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>44649.583333333336</v>
       </c>
@@ -816,7 +817,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>44648.583333333336</v>
       </c>
@@ -824,7 +825,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>44645.583333333336</v>
       </c>
@@ -832,7 +833,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>44644.583333333336</v>
       </c>
@@ -840,7 +841,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>44643.583333333336</v>
       </c>
@@ -848,7 +849,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>44642.583333333336</v>
       </c>
@@ -856,7 +857,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>44641.583333333336</v>
       </c>
@@ -864,7 +865,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>44638.583333333336</v>
       </c>
@@ -872,7 +873,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>44637.583333333336</v>
       </c>
@@ -880,7 +881,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>44636.583333333336</v>
       </c>
@@ -888,7 +889,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>44635.583333333336</v>
       </c>
@@ -896,7 +897,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>44634.583333333336</v>
       </c>
@@ -904,7 +905,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>44631.583333333336</v>
       </c>
@@ -912,7 +913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>44630.583333333336</v>
       </c>
@@ -920,7 +921,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>44629.583333333336</v>
       </c>
@@ -928,7 +929,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>44628.583333333336</v>
       </c>
@@ -936,7 +937,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>44627.583333333336</v>
       </c>
@@ -944,7 +945,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>44624.583333333336</v>
       </c>
@@ -952,7 +953,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>44623.583333333336</v>
       </c>
@@ -960,7 +961,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>44622.583333333336</v>
       </c>
@@ -968,7 +969,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>44621.583333333336</v>
       </c>
@@ -976,7 +977,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>44620.583333333336</v>
       </c>
@@ -984,7 +985,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44617.583333333336</v>
       </c>
@@ -992,7 +993,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>44616.583333333336</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>44615.583333333336</v>
       </c>
@@ -1008,7 +1009,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>44614.583333333336</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44610.583333333336</v>
       </c>
@@ -1024,7 +1025,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>44609.583333333336</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>44608.583333333336</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>44607.583333333336</v>
       </c>
@@ -1048,7 +1049,7 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>44606.583333333336</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>44603.583333333336</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>44602.583333333336</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>44601.583333333336</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>44600.583333333336</v>
       </c>
@@ -1088,7 +1089,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>44596.583333333336</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>1.93</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>44595.583333333336</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>44594.583333333336</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>44593.583333333336</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>44592.583333333336</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>44589.583333333336</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>44588.583333333336</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>44587.583333333336</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>44586.583333333336</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>44585.583333333336</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>44582.583333333336</v>
       </c>
@@ -1176,7 +1177,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>44581.583333333336</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>44580.583333333336</v>
       </c>
@@ -1192,7 +1193,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>44579.583333333336</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>44575.583333333336</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>44574.583333333336</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>44573.583333333336</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>44572.583333333336</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>44571.583333333336</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>44568.583333333336</v>
       </c>
@@ -1248,7 +1249,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>44567.583333333336</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>44566.583333333336</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>44565.583333333336</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>44564.583333333336</v>
       </c>
@@ -1280,597 +1281,227 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>44926.583333333336</v>
-      </c>
-      <c r="B116">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>44925.583333333336</v>
-      </c>
-      <c r="B117">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>44924.583333333336</v>
-      </c>
-      <c r="B118">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>44923.583333333336</v>
-      </c>
-      <c r="B119">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>44922.583333333336</v>
-      </c>
-      <c r="B120">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>44918.583333333336</v>
-      </c>
-      <c r="B121">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>44917.583333333336</v>
-      </c>
-      <c r="B122">
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>44916.583333333336</v>
-      </c>
-      <c r="B123">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>44915.583333333336</v>
-      </c>
-      <c r="B124">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>44912.583333333336</v>
-      </c>
-      <c r="B125">
-        <v>1.41</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>44911.583333333336</v>
-      </c>
-      <c r="B126">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>44910.583333333336</v>
-      </c>
-      <c r="B127">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
-        <v>44909.583333333336</v>
-      </c>
-      <c r="B128">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>44908.583333333336</v>
-      </c>
-      <c r="B129">
-        <v>1.42</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>44905.583333333336</v>
-      </c>
-      <c r="B130">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <v>44904.583333333336</v>
-      </c>
-      <c r="B131">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>44903.583333333336</v>
-      </c>
-      <c r="B132">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
-        <v>44902.583333333336</v>
-      </c>
-      <c r="B133">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
-        <v>44901.583333333336</v>
-      </c>
-      <c r="B134">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
-        <v>44898.583333333336</v>
-      </c>
-      <c r="B135">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
-        <v>44897.583333333336</v>
-      </c>
-      <c r="B136">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
-        <v>44896.583333333336</v>
-      </c>
-      <c r="B137">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <v>44895.583333333336</v>
-      </c>
-      <c r="B138">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
-        <v>44894.583333333336</v>
-      </c>
-      <c r="B139">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
-        <v>44891.583333333336</v>
-      </c>
-      <c r="B140">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>44889.583333333336</v>
-      </c>
-      <c r="B141">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
-        <v>44888.583333333336</v>
-      </c>
-      <c r="B142">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <v>44887.583333333336</v>
-      </c>
-      <c r="B143">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>44884.583333333336</v>
-      </c>
-      <c r="B144">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>44883.583333333336</v>
-      </c>
-      <c r="B145">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>44882.583333333336</v>
-      </c>
-      <c r="B146">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>44881.583333333336</v>
-      </c>
-      <c r="B147">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>44880.583333333336</v>
-      </c>
-      <c r="B148">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>44877.583333333336</v>
-      </c>
-      <c r="B149">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <v>44875.583333333336</v>
-      </c>
-      <c r="B150">
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
-        <v>44874.583333333336</v>
-      </c>
-      <c r="B151">
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
-        <v>44873.583333333336</v>
-      </c>
-      <c r="B152">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
-        <v>44870.583333333336</v>
-      </c>
-      <c r="B153">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>44869.583333333336</v>
-      </c>
-      <c r="B154">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>44868.583333333336</v>
-      </c>
-      <c r="B155">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>44867.583333333336</v>
-      </c>
-      <c r="B156">
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
-        <v>44866.583333333336</v>
-      </c>
-      <c r="B157">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <v>44863.583333333336</v>
-      </c>
-      <c r="B158">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <v>44862.583333333336</v>
-      </c>
-      <c r="B159">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>44861.583333333336</v>
-      </c>
-      <c r="B160">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
-        <v>44860.583333333336</v>
-      </c>
-      <c r="B161">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
-        <v>44859.583333333336</v>
-      </c>
-      <c r="B162">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
-        <v>44856.583333333336</v>
-      </c>
-      <c r="B163">
-        <v>1.66</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
-        <v>44855.583333333336</v>
-      </c>
-      <c r="B164">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
-        <v>44854.583333333336</v>
-      </c>
-      <c r="B165">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
-        <v>44853.583333333336</v>
-      </c>
-      <c r="B166">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
-        <v>44852.583333333336</v>
-      </c>
-      <c r="B167">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
-        <v>44849.583333333336</v>
-      </c>
-      <c r="B168">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
-        <v>44848.583333333336</v>
-      </c>
-      <c r="B169">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
-        <v>44847.583333333336</v>
-      </c>
-      <c r="B170">
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
-        <v>44846.583333333336</v>
-      </c>
-      <c r="B171">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
-        <v>44842.583333333336</v>
-      </c>
-      <c r="B172">
-        <v>1.61</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
-        <v>44841.583333333336</v>
-      </c>
-      <c r="B173">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
-        <v>44840.583333333336</v>
-      </c>
-      <c r="B174">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
-        <v>44839.583333333336</v>
-      </c>
-      <c r="B175">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
-        <v>44838.583333333336</v>
-      </c>
-      <c r="B176">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
-        <v>44835.583333333336</v>
-      </c>
-      <c r="B177">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
-        <v>44834.583333333336</v>
-      </c>
-      <c r="B178">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
-        <v>44833.583333333336</v>
-      </c>
-      <c r="B179">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
-        <v>44832.583333333336</v>
-      </c>
-      <c r="B180">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
-        <v>44831.583333333336</v>
-      </c>
-      <c r="B181">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
-        <v>44828.583333333336</v>
-      </c>
-      <c r="B182">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>44827.583333333336</v>
-      </c>
-      <c r="B183">
-        <v>1.41</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
-        <v>44826.583333333336</v>
-      </c>
-      <c r="B184">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
-        <v>44825.583333333336</v>
-      </c>
-      <c r="B185">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
-        <v>44824.583333333336</v>
-      </c>
-      <c r="B186">
-        <v>1.31</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
-        <v>44821.583333333336</v>
-      </c>
-      <c r="B187">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
-        <v>44820.583333333336</v>
-      </c>
-      <c r="B188">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
-        <v>44819.583333333336</v>
-      </c>
-      <c r="B189">
-        <v>1.31</v>
-      </c>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="1"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="1"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="1"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="1"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="1"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="1"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="1"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>